<commit_message>
Updates to annotations as I have progressed further through manually checking each one.
</commit_message>
<xml_diff>
--- a/prokka_outputs/Manually checked annotations/Nucleotide alignment Annotations.xlsx
+++ b/prokka_outputs/Manually checked annotations/Nucleotide alignment Annotations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Desktop/PhD/Project Work/Phylogenetic Study/Prokka and Orthofinder scripts and outputs/prokka_outputs/Manually checked annotations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/prokka_outputs/Manually checked annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA20B7C-3642-4C7E-9852-23BF746576ED}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{323B24B9-493D-43E3-B619-4288CC385390}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="198">
   <si>
     <t>Sequence Name</t>
   </si>
@@ -593,6 +593,30 @@
   </si>
   <si>
     <t>Present in reference genome but is longer. After a BLASTp search I found that the majority of sequences for this protien are equal to or closer in size to the longer version. As such, I amended the size of the prokka annotation to increase it to match the size of the reference genome.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matches with 24 other sequences with ~5 sharing &gt;80% identify. </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>This gene was included in the reference genome but was larger. BLASTp search found the majority of other  putative thymidine kinase genes match the size of the annotation included in the referenc genome. As such, I extended the gene.</t>
+  </si>
+  <si>
+    <t>Similar gene in reference genome (36 base pairs longer), but didn not stop with a stop codon like the annotation from Prokka so I kept the Prokka version.</t>
+  </si>
+  <si>
+    <t>Putative DNA-directed RNA polymerase II CDS or RPO2</t>
+  </si>
+  <si>
+    <t>Putative thymidine kinase. Matched with 'Deoxyribonucleoside kinase' from other megalocytivirus genotypes in GenBank.</t>
+  </si>
+  <si>
+    <t>Very similar to a gene in the annotated reference genome but a bit smaller. The version in the referenc egenome did not have a stop codon at the end so I have more trust in the Prokka annotation.</t>
+  </si>
+  <si>
+    <t>Hypothetical protein</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1127,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1131,13 +1155,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1211,6 +1228,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1533,8 +1554,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2037,44 +2058,44 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="11">
+    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7">
         <v>5174</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="7">
         <v>6631</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="7">
         <v>1458</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I15" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="12" t="s">
+      <c r="I15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2158,13 +2179,13 @@
       <c r="H18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K18" s="11" t="s">
+      <c r="I18" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L18" s="7" t="s">
@@ -2197,38 +2218,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="16" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="14">
+    <row r="20" spans="1:13" s="13" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="11">
         <v>8448</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="11">
         <v>8690</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="11">
         <v>243</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" s="15" t="s">
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="12" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2257,13 +2278,13 @@
       <c r="H21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K21" s="11" t="s">
+      <c r="I21" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L21" s="7" t="s">
@@ -2344,13 +2365,13 @@
       <c r="H24" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K24" s="11" t="s">
+      <c r="I24" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L24" s="7" t="s">
@@ -2408,13 +2429,13 @@
       <c r="H26" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="I26" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K26" s="11" t="s">
+      <c r="I26" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K26" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L26" s="7" t="s">
@@ -2472,13 +2493,13 @@
       <c r="H28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I28" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K28" s="11" t="s">
+      <c r="I28" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K28" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L28" s="7" t="s">
@@ -2513,13 +2534,13 @@
       <c r="H29" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I29" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K29" s="11" t="s">
+      <c r="I29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L29" s="7" t="s">
@@ -2577,13 +2598,13 @@
       <c r="H31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="11">
         <v>11309</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="14">
         <v>12268</v>
       </c>
-      <c r="K31" s="14">
+      <c r="K31" s="11">
         <v>960</v>
       </c>
       <c r="L31" s="7" t="s">
@@ -2641,13 +2662,13 @@
       <c r="H33" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I33" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K33" s="11" t="s">
+      <c r="I33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K33" s="7" t="s">
         <v>146</v>
       </c>
       <c r="L33" s="7" t="s">
@@ -2808,42 +2829,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="20" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B39" s="18" t="s">
+    <row r="39" spans="1:13" s="17" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="18">
+      <c r="C39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="15">
         <v>14322</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="15">
         <v>14513</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="15">
         <v>192</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19" t="s">
+      <c r="G39" s="16"/>
+      <c r="H39" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="18" t="s">
+      <c r="I39" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="J39" s="18" t="s">
+      <c r="J39" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="K39" s="18" t="s">
+      <c r="K39" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="L39" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" s="19" t="s">
+      <c r="L39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" s="16" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3200,7 +3221,7 @@
       <c r="H51" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="11">
         <v>22300</v>
       </c>
       <c r="J51" s="7">
@@ -3575,10 +3596,10 @@
       <c r="I63" s="7">
         <v>28593</v>
       </c>
-      <c r="J63" s="14">
+      <c r="J63" s="11">
         <v>28814</v>
       </c>
-      <c r="K63" s="14">
+      <c r="K63" s="11">
         <v>222</v>
       </c>
       <c r="L63" s="7" t="s">
@@ -3588,7 +3609,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>135</v>
       </c>
@@ -3607,11 +3628,29 @@
       <c r="F64" s="7">
         <v>603</v>
       </c>
+      <c r="G64" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K64" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L64" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>6</v>
       </c>
@@ -3634,7 +3673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>6</v>
       </c>
@@ -3657,7 +3696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>6</v>
       </c>
@@ -3680,7 +3719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>135</v>
       </c>
@@ -3699,11 +3738,29 @@
       <c r="F68" s="7">
         <v>567</v>
       </c>
+      <c r="G68" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I68" s="11">
+        <v>29447</v>
+      </c>
+      <c r="J68" s="7">
+        <v>30061</v>
+      </c>
+      <c r="K68" s="7">
+        <v>615</v>
+      </c>
       <c r="L68" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>6</v>
       </c>
@@ -3726,7 +3783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>135</v>
       </c>
@@ -3745,11 +3802,29 @@
       <c r="F70" s="7">
         <v>903</v>
       </c>
+      <c r="G70" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J70" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K70" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L70" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>6</v>
       </c>
@@ -3772,7 +3847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>135</v>
       </c>
@@ -3791,11 +3866,29 @@
       <c r="F72" s="7">
         <v>3135</v>
       </c>
+      <c r="G72" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K72" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L72" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>6</v>
       </c>
@@ -3818,7 +3911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>135</v>
       </c>
@@ -3837,11 +3930,29 @@
       <c r="F74" s="7">
         <v>1134</v>
       </c>
+      <c r="G74" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J74" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K74" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L74" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>6</v>
       </c>
@@ -3864,7 +3975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>135</v>
       </c>
@@ -3883,11 +3994,29 @@
       <c r="F76" s="7">
         <v>1026</v>
       </c>
+      <c r="G76" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J76" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K76" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L76" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>6</v>
       </c>
@@ -3910,7 +4039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>135</v>
       </c>
@@ -3929,11 +4058,29 @@
       <c r="F78" s="7">
         <v>1353</v>
       </c>
+      <c r="G78" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L78" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>6</v>
       </c>
@@ -3956,7 +4103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>135</v>
       </c>
@@ -3975,8 +4122,26 @@
       <c r="F80" s="7">
         <v>1437</v>
       </c>
+      <c r="G80" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I80" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J80" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K80" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L80" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -4020,6 +4185,9 @@
       </c>
       <c r="F82" s="7">
         <v>873</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="L82" s="7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updating annotations as I have progressed the manual annotation check.
</commit_message>
<xml_diff>
--- a/prokka_outputs/Manually checked annotations/Nucleotide alignment Annotations.xlsx
+++ b/prokka_outputs/Manually checked annotations/Nucleotide alignment Annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/prokka_outputs/Manually checked annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{323B24B9-493D-43E3-B619-4288CC385390}"/>
+  <xr:revisionPtr revIDLastSave="320" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{086324C8-D78B-4231-832D-88C830AC7B22}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
+    <workbookView xWindow="1332" yWindow="0" windowWidth="21432" windowHeight="13800" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
   </bookViews>
   <sheets>
     <sheet name="AF371960" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="198">
   <si>
     <t>Sequence Name</t>
   </si>
@@ -571,9 +571,6 @@
     <t>Putative ribonucleotide reductase small subunit CDS</t>
   </si>
   <si>
-    <t xml:space="preserve">Longer version of gene in reference genome. Having done a BALSTp search I found the majority of megalocytivirus Putative ribonucleotide reductase small subunits were 312 amino acids long (as opposed to 323 which was the Prokka annotated protein). As such i truncated the gene to match the reference gene annotation . </t>
-  </si>
-  <si>
     <t>Hypothetical Protein, maybe collagen-like protein</t>
   </si>
   <si>
@@ -617,6 +614,9 @@
   </si>
   <si>
     <t>Hypothetical protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Prokka annotatiuon had a longer version of the gene present in reference genome. Having done a BALSTp search I found the majority of megalocytivirus Putative ribonucleotide reductase small subunits were 312 amino acids long (as opposed to 323 which was the Prokka annotated protein). As such i truncated the gene to match the reference gene annotation . </t>
   </si>
 </sst>
 </file>
@@ -1554,8 +1554,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" topLeftCell="B76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3196,7 +3196,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>135</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>969</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>181</v>
@@ -3227,14 +3227,14 @@
       <c r="J51" s="7">
         <v>23238</v>
       </c>
-      <c r="K51" s="7">
-        <v>969</v>
+      <c r="K51" s="11">
+        <v>939</v>
       </c>
       <c r="L51" s="7" t="s">
         <v>11</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -3341,7 +3341,7 @@
         <v>151</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
@@ -3350,7 +3350,7 @@
         <v>11</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -3399,7 +3399,7 @@
         <v>148</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>146</v>
@@ -3463,7 +3463,7 @@
         <v>148</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>146</v>
@@ -3527,7 +3527,7 @@
         <v>148</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>146</v>
@@ -3591,7 +3591,7 @@
         <v>151</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I63" s="7">
         <v>28593</v>
@@ -3606,7 +3606,7 @@
         <v>9</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -3632,7 +3632,7 @@
         <v>151</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>146</v>
@@ -3647,7 +3647,7 @@
         <v>9</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -3739,10 +3739,10 @@
         <v>567</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I68" s="11">
         <v>29447</v>
@@ -3750,14 +3750,14 @@
       <c r="J68" s="7">
         <v>30061</v>
       </c>
-      <c r="K68" s="7">
+      <c r="K68" s="11">
         <v>615</v>
       </c>
       <c r="L68" s="7" t="s">
         <v>11</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
@@ -3803,10 +3803,10 @@
         <v>903</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>146</v>
@@ -3821,7 +3821,7 @@
         <v>9</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
@@ -3870,7 +3870,7 @@
         <v>148</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>146</v>
@@ -3931,10 +3931,10 @@
         <v>1134</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>146</v>
@@ -3949,7 +3949,7 @@
         <v>9</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
@@ -3995,10 +3995,10 @@
         <v>1026</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I76" s="7" t="s">
         <v>146</v>
@@ -4013,7 +4013,7 @@
         <v>11</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
@@ -4062,7 +4062,7 @@
         <v>148</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I78" s="7" t="s">
         <v>146</v>
@@ -4126,7 +4126,7 @@
         <v>148</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I80" s="7" t="s">
         <v>146</v>
@@ -4144,7 +4144,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>6</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>135</v>
       </c>
@@ -4189,11 +4189,26 @@
       <c r="G82" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="H82" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K82" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L82" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>6</v>
       </c>
@@ -4216,7 +4231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>135</v>
       </c>
@@ -4235,11 +4250,29 @@
       <c r="F84" s="7">
         <v>1140</v>
       </c>
+      <c r="G84" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J84" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K84" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L84" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>6</v>
       </c>
@@ -4262,7 +4295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>135</v>
       </c>
@@ -4281,11 +4314,26 @@
       <c r="F86" s="7">
         <v>1293</v>
       </c>
+      <c r="G86" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I86" s="7">
+        <v>41445</v>
+      </c>
+      <c r="J86" s="11">
+        <v>42788</v>
+      </c>
+      <c r="K86" s="11">
+        <v>1344</v>
+      </c>
       <c r="L86" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>6</v>
       </c>
@@ -4308,7 +4356,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>135</v>
       </c>
@@ -4331,7 +4379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
         <v>6</v>
       </c>
@@ -4354,7 +4402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>135</v>
       </c>
@@ -4377,7 +4425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>6</v>
       </c>
@@ -4400,7 +4448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
         <v>135</v>
       </c>
@@ -4423,7 +4471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
         <v>6</v>
       </c>
@@ -4446,7 +4494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
         <v>135</v>
       </c>
@@ -4469,7 +4517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>6</v>
       </c>
@@ -4492,7 +4540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
Updating annotations as I progress checking them manually
</commit_message>
<xml_diff>
--- a/prokka_outputs/Manually checked annotations/Nucleotide alignment Annotations.xlsx
+++ b/prokka_outputs/Manually checked annotations/Nucleotide alignment Annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/prokka_outputs/Manually checked annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{086324C8-D78B-4231-832D-88C830AC7B22}"/>
+  <xr:revisionPtr revIDLastSave="523" documentId="8_{F4CA95FD-ADD5-4464-8069-EE9EF4EC7303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D54E91CD-AFE5-4CB2-9D88-CDE0B9A80E4E}"/>
   <bookViews>
-    <workbookView xWindow="1332" yWindow="0" windowWidth="21432" windowHeight="13800" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{2726C256-0AC9-4A8B-B368-59495ADA43C2}"/>
   </bookViews>
   <sheets>
     <sheet name="AF371960" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="229">
   <si>
     <t>Sequence Name</t>
   </si>
@@ -617,13 +617,118 @@
   </si>
   <si>
     <t xml:space="preserve">The Prokka annotatiuon had a longer version of the gene present in reference genome. Having done a BALSTp search I found the majority of megalocytivirus Putative ribonucleotide reductase small subunits were 312 amino acids long (as opposed to 323 which was the Prokka annotated protein). As such i truncated the gene to match the reference gene annotation . </t>
+  </si>
+  <si>
+    <t>BLASTp search found the gene in the reference genome was equal to or closer majority of annotations.</t>
+  </si>
+  <si>
+    <t>Erv1/Alr family protein OR thiol oxidoreductase.</t>
+  </si>
+  <si>
+    <t>cytosine DNA methyltransferase </t>
+  </si>
+  <si>
+    <t>Hypothetical</t>
+  </si>
+  <si>
+    <t>Vascular endothelial growth factor </t>
+  </si>
+  <si>
+    <t>P142 </t>
+  </si>
+  <si>
+    <t>Not in Prokka annotatino but BLASTp returned one 99% identity match with only 43% coverage of the supposed gene. Decdied not to add to Prokka annotation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar gene in reference genome but the reference genome version was longer. BLASTp search found one match 99% identify and .90% coverage for Prokka version. The reference genome version had ~10 .90% identify matches with 99% coverage of the gene. Decedied to replace Prokka annotation with reference genome annotation.  </t>
+  </si>
+  <si>
+    <t>2-cysteine adaptor domain-containing protein</t>
+  </si>
+  <si>
+    <t>2-cysteine adaptor domain-containing protein </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exact match with reference sequence but also exact match / repeat with gene at minimun position 48633 and max position 49559. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Is this an issue or normal?</t>
+    </r>
+  </si>
+  <si>
+    <t>Covered the same position on the genome as two separate genes in the reference sequence. A BLASTp search of all three genes returned no matches for the two separate genes in the ref genome and ~12 matches with high % identify and coverage for the Prokka annotation. I decided to keep the Prokka annotation.</t>
+  </si>
+  <si>
+    <t>Replication factor </t>
+  </si>
+  <si>
+    <t>DNA-binding protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same gene, but difference sizes in ref genome and Prokka annotation. All matches for the gene in BLASTp (~20 matches) match the size of the ref genome annotation (1208 amino acids long). Decided to update Prokka annotation with the ref genome annotation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Macthes with &gt;99% identity and &gt;99% coverage in GenBank. Decided to keep.  </t>
+  </si>
+  <si>
+    <t>Putative NTPase CDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exact match with reference genome. </t>
+  </si>
+  <si>
+    <t>Putative RNA guanylytransferase CDS</t>
+  </si>
+  <si>
+    <t>RING-finger-containing E3 ubiquitin ligase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 BLASTp matches with ~10 matches with 90% identity and 100% query cover. </t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>~20 matches in Genbank but all are the size of the similar annotation in the reference genome which is larger than this one (153 amino acids in ref genome as oopsed to 63 in this Prokka annotation. Decided to remove.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No matched in Genbank so removed. </t>
+  </si>
+  <si>
+    <t>RING finger-containing E3 ubiquitin ligase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 matches in Genbank  but smaller than reference genome version which also returned ~100 matches and was the same size as the matches. The refernece genome annotation was 347 amino acids long as opposed to Prokka annotation which was 231 amino acids long. </t>
+  </si>
+  <si>
+    <t>Not present in reference genome but ~100 matched in GenBank and shared 80% identity with ~70% query cover with an antigen found in a few different susceptible finfish identified as 'CD83 antigen'</t>
+  </si>
+  <si>
+    <t>Returned ~100 matches with high level of identity on GenBank, and was the same size as the matches  (347 amino acids long as opposed to the version of this gene from the Prokka annotation which was 231 amino acids long). This family of proteins is associated with disease. It is adopted to regulate antiviral host response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 matches on GenBank. </t>
+  </si>
+  <si>
+    <t>Hypothetical protein OR CD276 antigen-like OR V-set domain-containing T-cell activation inhibitor 1</t>
+  </si>
+  <si>
+    <t>Many matched in GenBank. Shares identity with a number of genes found in finfish, some identified as  'CD276 antigen-like' or 'V-set domain-containing T-cell activation inhibitor 1'. Assume it has a role in regulating host's immune response to infection.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -775,6 +880,13 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1127,7 +1239,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1172,6 +1284,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1554,8 +1672,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A130" sqref="A130"/>
+      <selection pane="topRight" activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4295,7 +4415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>135</v>
       </c>
@@ -4332,6 +4452,9 @@
       <c r="L86" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="M86" s="2" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
@@ -4356,7 +4479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>135</v>
       </c>
@@ -4375,8 +4498,26 @@
       <c r="F88" s="7">
         <v>594</v>
       </c>
+      <c r="G88" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J88" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K88" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L88" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
@@ -4402,7 +4543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>135</v>
       </c>
@@ -4421,8 +4562,26 @@
       <c r="F90" s="7">
         <v>363</v>
       </c>
+      <c r="G90" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K90" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L90" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
@@ -4448,7 +4607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
         <v>135</v>
       </c>
@@ -4467,8 +4626,26 @@
       <c r="F92" s="7">
         <v>801</v>
       </c>
+      <c r="G92" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I92" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J92" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K92" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L92" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="M92" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
@@ -4494,7 +4671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
         <v>135</v>
       </c>
@@ -4513,8 +4690,26 @@
       <c r="F94" s="7">
         <v>915</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J94" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K94" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L94" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
@@ -4540,7 +4735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>135</v>
       </c>
@@ -4559,11 +4754,29 @@
       <c r="F96" s="7">
         <v>684</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J96" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K96" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L96" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M96" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
         <v>6</v>
       </c>
@@ -4586,7 +4799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
         <v>135</v>
       </c>
@@ -4605,11 +4818,29 @@
       <c r="F98" s="7">
         <v>264</v>
       </c>
+      <c r="G98" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K98" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L98" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M98" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
         <v>6</v>
       </c>
@@ -4632,7 +4863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>135</v>
       </c>
@@ -4651,11 +4882,29 @@
       <c r="F100" s="7">
         <v>345</v>
       </c>
+      <c r="G100" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I100" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J100" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K100" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L100" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M100" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>6</v>
       </c>
@@ -4678,7 +4927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>135</v>
       </c>
@@ -4697,11 +4946,29 @@
       <c r="F102" s="7">
         <v>171</v>
       </c>
+      <c r="G102" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K102" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L102" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M102" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>6</v>
       </c>
@@ -4724,7 +4991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
         <v>135</v>
       </c>
@@ -4743,11 +5010,29 @@
       <c r="F104" s="7">
         <v>429</v>
       </c>
+      <c r="G104" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H104" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="I104" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J104" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K104" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L104" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M104" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
         <v>6</v>
       </c>
@@ -4766,11 +5051,17 @@
       <c r="F105" s="7">
         <v>132</v>
       </c>
+      <c r="G105" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="L105" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M105" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>6</v>
       </c>
@@ -4793,7 +5084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>135</v>
       </c>
@@ -4812,11 +5103,29 @@
       <c r="F107" s="7">
         <v>453</v>
       </c>
+      <c r="G107" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J107" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K107" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L107" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M107" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>6</v>
       </c>
@@ -4839,7 +5148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>135</v>
       </c>
@@ -4858,11 +5167,29 @@
       <c r="F109" s="7">
         <v>192</v>
       </c>
+      <c r="G109" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I109" s="11">
+        <v>48405</v>
+      </c>
+      <c r="J109" s="11">
+        <v>48620</v>
+      </c>
+      <c r="K109" s="11">
+        <v>216</v>
+      </c>
       <c r="L109" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M109" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
         <v>6</v>
       </c>
@@ -4885,7 +5212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
         <v>135</v>
       </c>
@@ -4904,11 +5231,29 @@
       <c r="F111" s="7">
         <v>927</v>
       </c>
+      <c r="G111" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I111" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L111" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M111" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
         <v>6</v>
       </c>
@@ -4931,7 +5276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>135</v>
       </c>
@@ -4950,11 +5295,29 @@
       <c r="F113" s="7">
         <v>927</v>
       </c>
+      <c r="G113" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I113" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L113" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M113" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
         <v>6</v>
       </c>
@@ -4977,7 +5340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
         <v>135</v>
       </c>
@@ -4996,11 +5359,29 @@
       <c r="F115" s="7">
         <v>648</v>
       </c>
+      <c r="G115" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K115" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L115" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M115" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
         <v>6</v>
       </c>
@@ -5023,7 +5404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
         <v>135</v>
       </c>
@@ -5042,11 +5423,29 @@
       <c r="F117" s="7">
         <v>261</v>
       </c>
+      <c r="G117" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I117" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J117" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K117" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L117" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M117" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
         <v>6</v>
       </c>
@@ -5069,7 +5468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>135</v>
       </c>
@@ -5088,11 +5487,29 @@
       <c r="F119" s="7">
         <v>300</v>
       </c>
+      <c r="G119" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I119" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K119" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L119" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M119" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>135</v>
       </c>
@@ -5111,11 +5528,29 @@
       <c r="F120" s="7">
         <v>666</v>
       </c>
+      <c r="G120" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I120" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J120" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K120" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L120" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M120" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>6</v>
       </c>
@@ -5138,7 +5573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
         <v>6</v>
       </c>
@@ -5161,7 +5596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>6</v>
       </c>
@@ -5184,7 +5619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>135</v>
       </c>
@@ -5203,11 +5638,29 @@
       <c r="F124" s="7">
         <v>804</v>
       </c>
+      <c r="G124" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I124" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J124" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K124" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L124" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M124" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>6</v>
       </c>
@@ -5230,7 +5683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>135</v>
       </c>
@@ -5249,11 +5702,29 @@
       <c r="F126" s="7">
         <v>3324</v>
       </c>
+      <c r="G126" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I126" s="7">
+        <v>53159</v>
+      </c>
+      <c r="J126" s="11">
+        <v>56785</v>
+      </c>
+      <c r="K126" s="11">
+        <v>3627</v>
+      </c>
       <c r="L126" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M126" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
         <v>135</v>
       </c>
@@ -5272,11 +5743,29 @@
       <c r="F127" s="7">
         <v>369</v>
       </c>
+      <c r="G127" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I127" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J127" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K127" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L127" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M127" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
         <v>6</v>
       </c>
@@ -5299,7 +5788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
         <v>135</v>
       </c>
@@ -5318,11 +5807,29 @@
       <c r="F129" s="7">
         <v>2649</v>
       </c>
+      <c r="G129" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I129" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L129" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M129" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
         <v>6</v>
       </c>
@@ -5345,7 +5852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>135</v>
       </c>
@@ -5364,11 +5871,29 @@
       <c r="F131" s="7">
         <v>1476</v>
       </c>
+      <c r="G131" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I131" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J131" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K131" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L131" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M131" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
         <v>6</v>
       </c>
@@ -5387,11 +5912,29 @@
       <c r="F132" s="7">
         <v>462</v>
       </c>
-      <c r="L132" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G132" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="H132" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="I132" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="J132" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="K132" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="L132" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M132" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>135</v>
       </c>
@@ -5410,11 +5953,29 @@
       <c r="F133" s="7">
         <v>189</v>
       </c>
-      <c r="L133" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G133" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H133" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="I133" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="J133" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="K133" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L133" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M133" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>135</v>
       </c>
@@ -5433,11 +5994,29 @@
       <c r="F134" s="7">
         <v>294</v>
       </c>
-      <c r="L134" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G134" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H134" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="I134" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="J134" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="K134" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L134" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M134" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>6</v>
       </c>
@@ -5456,11 +6035,29 @@
       <c r="F135" s="7">
         <v>1044</v>
       </c>
-      <c r="L135" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G135" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H135" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="I135" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="J135" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="K135" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="L135" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M135" s="18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>135</v>
       </c>
@@ -5479,11 +6076,29 @@
       <c r="F136" s="7">
         <v>693</v>
       </c>
-      <c r="L136" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G136" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H136" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="I136" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="J136" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="K136" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L136" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M136" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>6</v>
       </c>
@@ -5506,7 +6121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>135</v>
       </c>
@@ -5525,11 +6140,29 @@
       <c r="F138" s="7">
         <v>585</v>
       </c>
+      <c r="G138" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I138" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J138" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K138" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L138" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M138" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>6</v>
       </c>
@@ -5552,7 +6185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>135</v>
       </c>
@@ -5571,11 +6204,29 @@
       <c r="F140" s="7">
         <v>1434</v>
       </c>
+      <c r="G140" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I140" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J140" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K140" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L140" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M140" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>6</v>
       </c>
@@ -5598,7 +6249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>135</v>
       </c>
@@ -5617,11 +6268,29 @@
       <c r="F142" s="7">
         <v>666</v>
       </c>
+      <c r="G142" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I142" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J142" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K142" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="L142" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M142" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>135</v>
       </c>
@@ -5644,7 +6313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>6</v>
       </c>

</xml_diff>